<commit_message>
ajusto validación de excel
</commit_message>
<xml_diff>
--- a/AsistManager/wwwroot/xlsx/registros.xlsx
+++ b/AsistManager/wwwroot/xlsx/registros.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sampi\Desktop\Laburo\Axcess\AsistManager\AsistManager\AsistManager\wwwroot\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42E45CE-811C-4C0F-816D-021B2C566686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D2F89-0916-4202-80F6-C0639650678D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,8 +443,8 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{42C176A8-E694-4A4E-855D-FEA27A9CB498}">
-      <formula1>8</formula1>
+    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{42C176A8-E694-4A4E-855D-FEA27A9CB498}">
+      <formula1>7</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576 H1:H1048576" xr:uid="{69550E26-9647-43E3-A548-CF2B02E8A5FA}">
       <formula1>2</formula1>
@@ -452,9 +452,6 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C1 C4 C6:C1048576" listDataValidation="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>